<commit_message>
-No dropdown available with db stocks to plot
</commit_message>
<xml_diff>
--- a/TestWebApp/the_site/results.xlsx
+++ b/TestWebApp/the_site/results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Main" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Main" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -24,7 +24,7 @@
     <t>Company A - Share Value</t>
   </si>
   <si>
-    <t>2019-02-26 10:28:34</t>
+    <t>2019-02-26 15:46:04</t>
   </si>
   <si>
     <t>2019-01-31</t>

</xml_diff>

<commit_message>
full functional stocks graphing app
</commit_message>
<xml_diff>
--- a/TestWebApp/the_site/results.xlsx
+++ b/TestWebApp/the_site/results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="234">
   <si>
     <t>Company A - Date</t>
   </si>
@@ -370,6 +370,354 @@
   </si>
   <si>
     <t>2009-07-31</t>
+  </si>
+  <si>
+    <t>2009-06-30</t>
+  </si>
+  <si>
+    <t>2009-05-29</t>
+  </si>
+  <si>
+    <t>2009-04-30</t>
+  </si>
+  <si>
+    <t>2009-03-31</t>
+  </si>
+  <si>
+    <t>2009-02-27</t>
+  </si>
+  <si>
+    <t>2009-01-30</t>
+  </si>
+  <si>
+    <t>2008-12-31</t>
+  </si>
+  <si>
+    <t>2008-11-28</t>
+  </si>
+  <si>
+    <t>2008-10-31</t>
+  </si>
+  <si>
+    <t>2008-09-30</t>
+  </si>
+  <si>
+    <t>2008-08-29</t>
+  </si>
+  <si>
+    <t>2008-07-31</t>
+  </si>
+  <si>
+    <t>2008-06-30</t>
+  </si>
+  <si>
+    <t>2008-05-30</t>
+  </si>
+  <si>
+    <t>2008-04-30</t>
+  </si>
+  <si>
+    <t>2008-03-31</t>
+  </si>
+  <si>
+    <t>2008-02-29</t>
+  </si>
+  <si>
+    <t>2008-01-31</t>
+  </si>
+  <si>
+    <t>2007-12-31</t>
+  </si>
+  <si>
+    <t>2007-11-30</t>
+  </si>
+  <si>
+    <t>2007-10-31</t>
+  </si>
+  <si>
+    <t>2007-09-28</t>
+  </si>
+  <si>
+    <t>2007-08-31</t>
+  </si>
+  <si>
+    <t>2007-07-31</t>
+  </si>
+  <si>
+    <t>2007-06-29</t>
+  </si>
+  <si>
+    <t>2007-05-31</t>
+  </si>
+  <si>
+    <t>2007-04-30</t>
+  </si>
+  <si>
+    <t>2007-03-30</t>
+  </si>
+  <si>
+    <t>2007-02-28</t>
+  </si>
+  <si>
+    <t>2007-01-31</t>
+  </si>
+  <si>
+    <t>2006-12-29</t>
+  </si>
+  <si>
+    <t>2006-11-30</t>
+  </si>
+  <si>
+    <t>2006-10-31</t>
+  </si>
+  <si>
+    <t>2006-09-29</t>
+  </si>
+  <si>
+    <t>2006-08-31</t>
+  </si>
+  <si>
+    <t>2006-07-31</t>
+  </si>
+  <si>
+    <t>2006-06-30</t>
+  </si>
+  <si>
+    <t>2006-05-31</t>
+  </si>
+  <si>
+    <t>2006-04-28</t>
+  </si>
+  <si>
+    <t>2006-03-31</t>
+  </si>
+  <si>
+    <t>2006-02-28</t>
+  </si>
+  <si>
+    <t>2006-01-31</t>
+  </si>
+  <si>
+    <t>2005-12-30</t>
+  </si>
+  <si>
+    <t>2005-11-30</t>
+  </si>
+  <si>
+    <t>2005-10-31</t>
+  </si>
+  <si>
+    <t>2005-09-30</t>
+  </si>
+  <si>
+    <t>2005-08-31</t>
+  </si>
+  <si>
+    <t>2005-07-29</t>
+  </si>
+  <si>
+    <t>2005-06-30</t>
+  </si>
+  <si>
+    <t>2005-05-31</t>
+  </si>
+  <si>
+    <t>2005-04-29</t>
+  </si>
+  <si>
+    <t>2005-03-31</t>
+  </si>
+  <si>
+    <t>2005-02-28</t>
+  </si>
+  <si>
+    <t>2005-01-31</t>
+  </si>
+  <si>
+    <t>2004-12-31</t>
+  </si>
+  <si>
+    <t>2004-11-30</t>
+  </si>
+  <si>
+    <t>2004-10-29</t>
+  </si>
+  <si>
+    <t>2004-09-30</t>
+  </si>
+  <si>
+    <t>2004-08-31</t>
+  </si>
+  <si>
+    <t>2004-07-30</t>
+  </si>
+  <si>
+    <t>2004-06-30</t>
+  </si>
+  <si>
+    <t>2004-05-28</t>
+  </si>
+  <si>
+    <t>2004-04-30</t>
+  </si>
+  <si>
+    <t>2004-03-31</t>
+  </si>
+  <si>
+    <t>2004-02-27</t>
+  </si>
+  <si>
+    <t>2004-01-30</t>
+  </si>
+  <si>
+    <t>2003-12-31</t>
+  </si>
+  <si>
+    <t>2003-11-28</t>
+  </si>
+  <si>
+    <t>2003-10-31</t>
+  </si>
+  <si>
+    <t>2003-09-30</t>
+  </si>
+  <si>
+    <t>2003-08-29</t>
+  </si>
+  <si>
+    <t>2003-07-31</t>
+  </si>
+  <si>
+    <t>2003-06-30</t>
+  </si>
+  <si>
+    <t>2003-05-30</t>
+  </si>
+  <si>
+    <t>2003-04-30</t>
+  </si>
+  <si>
+    <t>2003-03-31</t>
+  </si>
+  <si>
+    <t>2003-02-28</t>
+  </si>
+  <si>
+    <t>2003-01-31</t>
+  </si>
+  <si>
+    <t>2002-12-31</t>
+  </si>
+  <si>
+    <t>2002-11-29</t>
+  </si>
+  <si>
+    <t>2002-10-31</t>
+  </si>
+  <si>
+    <t>2002-09-30</t>
+  </si>
+  <si>
+    <t>2002-08-30</t>
+  </si>
+  <si>
+    <t>2002-07-31</t>
+  </si>
+  <si>
+    <t>2002-06-28</t>
+  </si>
+  <si>
+    <t>2002-05-31</t>
+  </si>
+  <si>
+    <t>2002-04-30</t>
+  </si>
+  <si>
+    <t>2002-03-28</t>
+  </si>
+  <si>
+    <t>2002-02-28</t>
+  </si>
+  <si>
+    <t>2002-01-31</t>
+  </si>
+  <si>
+    <t>2001-12-31</t>
+  </si>
+  <si>
+    <t>2001-11-30</t>
+  </si>
+  <si>
+    <t>2001-10-31</t>
+  </si>
+  <si>
+    <t>2001-09-28</t>
+  </si>
+  <si>
+    <t>2001-08-31</t>
+  </si>
+  <si>
+    <t>2001-07-31</t>
+  </si>
+  <si>
+    <t>2001-06-29</t>
+  </si>
+  <si>
+    <t>2001-05-31</t>
+  </si>
+  <si>
+    <t>2001-04-30</t>
+  </si>
+  <si>
+    <t>2001-03-30</t>
+  </si>
+  <si>
+    <t>2001-02-28</t>
+  </si>
+  <si>
+    <t>2001-01-31</t>
+  </si>
+  <si>
+    <t>2000-12-29</t>
+  </si>
+  <si>
+    <t>2000-11-30</t>
+  </si>
+  <si>
+    <t>2000-10-31</t>
+  </si>
+  <si>
+    <t>2000-09-29</t>
+  </si>
+  <si>
+    <t>2000-08-31</t>
+  </si>
+  <si>
+    <t>2000-07-31</t>
+  </si>
+  <si>
+    <t>2000-06-30</t>
+  </si>
+  <si>
+    <t>2000-05-31</t>
+  </si>
+  <si>
+    <t>2000-04-28</t>
+  </si>
+  <si>
+    <t>2000-03-31</t>
+  </si>
+  <si>
+    <t>2000-02-29</t>
+  </si>
+  <si>
+    <t>2000-01-31</t>
+  </si>
+  <si>
+    <t>1999-12-31</t>
+  </si>
+  <si>
+    <t>1999-11-30</t>
   </si>
 </sst>
 </file>
@@ -741,7 +1089,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D117"/>
+  <dimension ref="A1:D233"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -770,7 +1118,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="4" t="n">
-        <v>25.43</v>
+        <v>218.31</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -778,7 +1126,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="4" t="n">
-        <v>24.73</v>
+        <v>226.74</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -786,7 +1134,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="4" t="n">
-        <v>24.75</v>
+        <v>237.87</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -794,7 +1142,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="4" t="n">
-        <v>24.32</v>
+        <v>244.46</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -802,7 +1150,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="4" t="n">
-        <v>23.53</v>
+        <v>242.81</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -810,7 +1158,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="4" t="n">
-        <v>22.37</v>
+        <v>234.32</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -818,7 +1166,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="4" t="n">
-        <v>21.6</v>
+        <v>227.24</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -826,7 +1174,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="4" t="n">
-        <v>21.19</v>
+        <v>220.71</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -834,7 +1182,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="4" t="n">
-        <v>20.75</v>
+        <v>214.29</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -842,7 +1190,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="4" t="n">
-        <v>21.09</v>
+        <v>205.11</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -850,7 +1198,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="4" t="n">
-        <v>21.37</v>
+        <v>197.15</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -858,7 +1206,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="4" t="n">
-        <v>22</v>
+        <v>188.78</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -866,7 +1214,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="4" t="n">
-        <v>22.51</v>
+        <v>175.06</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -874,7 +1222,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="4" t="n">
-        <v>22.98</v>
+        <v>162.1</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -882,7 +1230,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="4" t="n">
-        <v>23.66</v>
+        <v>152.91</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -890,7 +1238,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="4" t="n">
-        <v>24.62</v>
+        <v>144.03</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -898,7 +1246,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="4" t="n">
-        <v>25.54</v>
+        <v>133.54</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -906,7 +1254,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="4" t="n">
-        <v>26.15</v>
+        <v>124.67</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -914,7 +1262,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="4" t="n">
-        <v>26.55</v>
+        <v>114.81</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -922,7 +1270,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="4" t="n">
-        <v>26.84</v>
+        <v>105.45</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -930,7 +1278,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="4" t="n">
-        <v>26.79</v>
+        <v>97.09</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -938,7 +1286,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="4" t="n">
-        <v>26.66</v>
+        <v>88.31999999999999</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -946,7 +1294,7 @@
         <v>24</v>
       </c>
       <c r="B24" s="4" t="n">
-        <v>26.24</v>
+        <v>82.52</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -954,7 +1302,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="4" t="n">
-        <v>26.07</v>
+        <v>76.28</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -962,7 +1310,7 @@
         <v>26</v>
       </c>
       <c r="B26" s="4" t="n">
-        <v>25.93</v>
+        <v>69.48999999999999</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -970,7 +1318,7 @@
         <v>27</v>
       </c>
       <c r="B27" s="4" t="n">
-        <v>25.83</v>
+        <v>61.97</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -978,7 +1326,7 @@
         <v>28</v>
       </c>
       <c r="B28" s="4" t="n">
-        <v>25.61</v>
+        <v>54.67</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -986,7 +1334,7 @@
         <v>29</v>
       </c>
       <c r="B29" s="4" t="n">
-        <v>25.66</v>
+        <v>48.39</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -994,7 +1342,7 @@
         <v>30</v>
       </c>
       <c r="B30" s="4" t="n">
-        <v>25.64</v>
+        <v>44.48</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1002,7 +1350,7 @@
         <v>31</v>
       </c>
       <c r="B31" s="4" t="n">
-        <v>25.98</v>
+        <v>40.83</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1010,7 +1358,7 @@
         <v>32</v>
       </c>
       <c r="B32" s="4" t="n">
-        <v>26.25</v>
+        <v>37.53</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1018,7 +1366,7 @@
         <v>33</v>
       </c>
       <c r="B33" s="4" t="n">
-        <v>26.23</v>
+        <v>34.26</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1026,7 +1374,7 @@
         <v>34</v>
       </c>
       <c r="B34" s="4" t="n">
-        <v>26.34</v>
+        <v>31.77</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1034,7 +1382,7 @@
         <v>35</v>
       </c>
       <c r="B35" s="4" t="n">
-        <v>26.69</v>
+        <v>29.13</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1042,7 +1390,7 @@
         <v>36</v>
       </c>
       <c r="B36" s="4" t="n">
-        <v>27.14</v>
+        <v>27.61</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1050,7 +1398,7 @@
         <v>37</v>
       </c>
       <c r="B37" s="4" t="n">
-        <v>27.61</v>
+        <v>26.29</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1058,7 +1406,7 @@
         <v>38</v>
       </c>
       <c r="B38" s="4" t="n">
-        <v>28.15</v>
+        <v>25.39</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1066,7 +1414,7 @@
         <v>39</v>
       </c>
       <c r="B39" s="4" t="n">
-        <v>28.41</v>
+        <v>24.56</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1074,7 +1422,7 @@
         <v>40</v>
       </c>
       <c r="B40" s="4" t="n">
-        <v>29</v>
+        <v>23.53</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1082,7 +1430,7 @@
         <v>41</v>
       </c>
       <c r="B41" s="4" t="n">
-        <v>28.84</v>
+        <v>22.26</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1090,7 +1438,7 @@
         <v>42</v>
       </c>
       <c r="B42" s="4" t="n">
-        <v>29.45</v>
+        <v>21.43</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1098,7 +1446,7 @@
         <v>43</v>
       </c>
       <c r="B43" s="4" t="n">
-        <v>30.41</v>
+        <v>21.05</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1106,7 +1454,7 @@
         <v>44</v>
       </c>
       <c r="B44" s="4" t="n">
-        <v>31.41</v>
+        <v>20.87</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1114,7 +1462,7 @@
         <v>45</v>
       </c>
       <c r="B45" s="4" t="n">
-        <v>32.11</v>
+        <v>20.71</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1122,7 +1470,7 @@
         <v>46</v>
       </c>
       <c r="B46" s="4" t="n">
-        <v>33.29</v>
+        <v>20.6</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1130,7 +1478,7 @@
         <v>47</v>
       </c>
       <c r="B47" s="4" t="n">
-        <v>38.44</v>
+        <v>20.12</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1138,7 +1486,7 @@
         <v>48</v>
       </c>
       <c r="B48" s="4" t="n">
-        <v>42.69</v>
+        <v>19.73</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1146,7 +1494,7 @@
         <v>49</v>
       </c>
       <c r="B49" s="4" t="n">
-        <v>47.24</v>
+        <v>19.54</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1154,7 +1502,7 @@
         <v>50</v>
       </c>
       <c r="B50" s="4" t="n">
-        <v>51.23</v>
+        <v>19.21</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1162,7 +1510,7 @@
         <v>51</v>
       </c>
       <c r="B51" s="4" t="n">
-        <v>56.17</v>
+        <v>19.13</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1170,7 +1518,7 @@
         <v>52</v>
       </c>
       <c r="B52" s="4" t="n">
-        <v>60.46</v>
+        <v>18.91</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1178,7 +1526,7 @@
         <v>53</v>
       </c>
       <c r="B53" s="4" t="n">
-        <v>64.45999999999999</v>
+        <v>18.41</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1186,7 +1534,7 @@
         <v>54</v>
       </c>
       <c r="B54" s="4" t="n">
-        <v>69.28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1194,7 +1542,7 @@
         <v>55</v>
       </c>
       <c r="B55" s="4" t="n">
-        <v>73.67</v>
+        <v>17.7</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1202,7 +1550,7 @@
         <v>56</v>
       </c>
       <c r="B56" s="4" t="n">
-        <v>77.59</v>
+        <v>17.28</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1210,7 +1558,7 @@
         <v>57</v>
       </c>
       <c r="B57" s="4" t="n">
-        <v>77.14</v>
+        <v>17.09</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1218,7 +1566,7 @@
         <v>58</v>
       </c>
       <c r="B58" s="4" t="n">
-        <v>77.05</v>
+        <v>16.72</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1226,7 +1574,7 @@
         <v>59</v>
       </c>
       <c r="B59" s="4" t="n">
-        <v>76.81999999999999</v>
+        <v>16.26</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1234,7 +1582,7 @@
         <v>60</v>
       </c>
       <c r="B60" s="4" t="n">
-        <v>76.83</v>
+        <v>15.8</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -1242,7 +1590,7 @@
         <v>61</v>
       </c>
       <c r="B61" s="4" t="n">
-        <v>76.12</v>
+        <v>15.4</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1250,7 +1598,7 @@
         <v>62</v>
       </c>
       <c r="B62" s="4" t="n">
-        <v>75.58</v>
+        <v>14.98</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -1258,7 +1606,7 @@
         <v>63</v>
       </c>
       <c r="B63" s="4" t="n">
-        <v>75.18000000000001</v>
+        <v>14.68</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1266,7 +1614,7 @@
         <v>64</v>
       </c>
       <c r="B64" s="4" t="n">
-        <v>73.23</v>
+        <v>14.34</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1274,7 +1622,7 @@
         <v>65</v>
       </c>
       <c r="B65" s="4" t="n">
-        <v>71.51000000000001</v>
+        <v>14.03</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1282,7 +1630,7 @@
         <v>66</v>
       </c>
       <c r="B66" s="4" t="n">
-        <v>69.29000000000001</v>
+        <v>13.76</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -1290,7 +1638,7 @@
         <v>67</v>
       </c>
       <c r="B67" s="4" t="n">
-        <v>67.06999999999999</v>
+        <v>13.41</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -1298,7 +1646,7 @@
         <v>68</v>
       </c>
       <c r="B68" s="4" t="n">
-        <v>65.36</v>
+        <v>13.13</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -1306,7 +1654,7 @@
         <v>69</v>
       </c>
       <c r="B69" s="4" t="n">
-        <v>63.71</v>
+        <v>13.03</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -1314,7 +1662,7 @@
         <v>70</v>
       </c>
       <c r="B70" s="4" t="n">
-        <v>61.81</v>
+        <v>12.99</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -1322,7 +1670,7 @@
         <v>71</v>
       </c>
       <c r="B71" s="4" t="n">
-        <v>59.45</v>
+        <v>12.9</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -1330,7 +1678,7 @@
         <v>72</v>
       </c>
       <c r="B72" s="4" t="n">
-        <v>57.32</v>
+        <v>12.92</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -1338,7 +1686,7 @@
         <v>73</v>
       </c>
       <c r="B73" s="4" t="n">
-        <v>54.98</v>
+        <v>12.85</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -1346,7 +1694,7 @@
         <v>74</v>
       </c>
       <c r="B74" s="4" t="n">
-        <v>53.58</v>
+        <v>12.89</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -1354,7 +1702,7 @@
         <v>75</v>
       </c>
       <c r="B75" s="4" t="n">
-        <v>51.88</v>
+        <v>13.19</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -1362,7 +1710,7 @@
         <v>76</v>
       </c>
       <c r="B76" s="4" t="n">
-        <v>50.22</v>
+        <v>13.45</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -1370,7 +1718,7 @@
         <v>77</v>
       </c>
       <c r="B77" s="4" t="n">
-        <v>48.5</v>
+        <v>13.74</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -1378,7 +1726,7 @@
         <v>78</v>
       </c>
       <c r="B78" s="4" t="n">
-        <v>46.84</v>
+        <v>13.96</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -1386,7 +1734,7 @@
         <v>79</v>
       </c>
       <c r="B79" s="4" t="n">
-        <v>44.98</v>
+        <v>14.17</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -1394,7 +1742,7 @@
         <v>80</v>
       </c>
       <c r="B80" s="4" t="n">
-        <v>43.63</v>
+        <v>14.22</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -1402,7 +1750,7 @@
         <v>81</v>
       </c>
       <c r="B81" s="4" t="n">
-        <v>42.46</v>
+        <v>14.09</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -1410,7 +1758,7 @@
         <v>82</v>
       </c>
       <c r="B82" s="4" t="n">
-        <v>41.41</v>
+        <v>14.05</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -1418,7 +1766,7 @@
         <v>83</v>
       </c>
       <c r="B83" s="4" t="n">
-        <v>40.4</v>
+        <v>14.25</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -1426,7 +1774,7 @@
         <v>84</v>
       </c>
       <c r="B84" s="4" t="n">
-        <v>39.1</v>
+        <v>14.55</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -1434,7 +1782,7 @@
         <v>85</v>
       </c>
       <c r="B85" s="4" t="n">
-        <v>38.26</v>
+        <v>15.01</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -1442,7 +1790,7 @@
         <v>86</v>
       </c>
       <c r="B86" s="4" t="n">
-        <v>37.87</v>
+        <v>15.53</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -1450,7 +1798,7 @@
         <v>87</v>
       </c>
       <c r="B87" s="4" t="n">
-        <v>37.47</v>
+        <v>15.91</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -1458,7 +1806,7 @@
         <v>88</v>
       </c>
       <c r="B88" s="4" t="n">
-        <v>37.46</v>
+        <v>16.75</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -1466,7 +1814,7 @@
         <v>89</v>
       </c>
       <c r="B89" s="4" t="n">
-        <v>37.09</v>
+        <v>17.61</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -1474,7 +1822,7 @@
         <v>90</v>
       </c>
       <c r="B90" s="4" t="n">
-        <v>36.96</v>
+        <v>17.73</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -1482,7 +1830,7 @@
         <v>91</v>
       </c>
       <c r="B91" s="4" t="n">
-        <v>37.04</v>
+        <v>17.89</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -1490,7 +1838,7 @@
         <v>92</v>
       </c>
       <c r="B92" s="4" t="n">
-        <v>37</v>
+        <v>17.75</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -1498,7 +1846,7 @@
         <v>93</v>
       </c>
       <c r="B93" s="4" t="n">
-        <v>37.19</v>
+        <v>17.52</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -1506,7 +1854,7 @@
         <v>94</v>
       </c>
       <c r="B94" s="4" t="n">
-        <v>36.94</v>
+        <v>16.87</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -1514,7 +1862,7 @@
         <v>95</v>
       </c>
       <c r="B95" s="4" t="n">
-        <v>36.57</v>
+        <v>15.81</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -1522,7 +1870,7 @@
         <v>96</v>
       </c>
       <c r="B96" s="4" t="n">
-        <v>35.7</v>
+        <v>14.79</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -1530,7 +1878,7 @@
         <v>97</v>
       </c>
       <c r="B97" s="4" t="n">
-        <v>35.32</v>
+        <v>14.22</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -1538,7 +1886,7 @@
         <v>98</v>
       </c>
       <c r="B98" s="4" t="n">
-        <v>34.88</v>
+        <v>13.53</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -1546,7 +1894,7 @@
         <v>99</v>
       </c>
       <c r="B99" s="4" t="n">
-        <v>34.43</v>
+        <v>12.86</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -1554,7 +1902,7 @@
         <v>100</v>
       </c>
       <c r="B100" s="4" t="n">
-        <v>33.41</v>
+        <v>12.93</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -1562,7 +1910,7 @@
         <v>101</v>
       </c>
       <c r="B101" s="4" t="n">
-        <v>32.48</v>
+        <v>13.09</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -1570,7 +1918,7 @@
         <v>102</v>
       </c>
       <c r="B102" s="4" t="n">
-        <v>31.24</v>
+        <v>13.73</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -1578,7 +1926,7 @@
         <v>103</v>
       </c>
       <c r="B103" s="4" t="n">
-        <v>30.25</v>
+        <v>13.86</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -1586,7 +1934,7 @@
         <v>104</v>
       </c>
       <c r="B104" s="4" t="n">
-        <v>29.23</v>
+        <v>14.11</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -1594,7 +1942,7 @@
         <v>105</v>
       </c>
       <c r="B105" s="4" t="n">
-        <v>28.38</v>
+        <v>14.67</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -1602,7 +1950,7 @@
         <v>106</v>
       </c>
       <c r="B106" s="4" t="n">
-        <v>27.65</v>
+        <v>15.1</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -1610,7 +1958,7 @@
         <v>107</v>
       </c>
       <c r="B107" s="4" t="n">
-        <v>26.76</v>
+        <v>15.12</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -1618,7 +1966,7 @@
         <v>108</v>
       </c>
       <c r="B108" s="4" t="n">
-        <v>25.44</v>
+        <v>14.68</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -1626,7 +1974,7 @@
         <v>109</v>
       </c>
       <c r="B109" s="4" t="n">
-        <v>24.58</v>
+        <v>13.99</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -1634,7 +1982,7 @@
         <v>110</v>
       </c>
       <c r="B110" s="4" t="n">
-        <v>23.67</v>
+        <v>13.51</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -1642,7 +1990,7 @@
         <v>111</v>
       </c>
       <c r="B111" s="4" t="n">
-        <v>22.46</v>
+        <v>12.94</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -1650,7 +1998,7 @@
         <v>112</v>
       </c>
       <c r="B112" s="4" t="n">
-        <v>21.23</v>
+        <v>11.88</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -1658,7 +2006,7 @@
         <v>113</v>
       </c>
       <c r="B113" s="4" t="n">
-        <v>19.82</v>
+        <v>11.36</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -1666,7 +2014,7 @@
         <v>114</v>
       </c>
       <c r="B114" s="4" t="n">
-        <v>18.76</v>
+        <v>10.97</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -1674,7 +2022,7 @@
         <v>115</v>
       </c>
       <c r="B115" s="4" t="n">
-        <v>17.42</v>
+        <v>10.19</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -1682,7 +2030,7 @@
         <v>116</v>
       </c>
       <c r="B116" s="4" t="n">
-        <v>16.39</v>
+        <v>9.630000000000001</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -1690,7 +2038,935 @@
         <v>117</v>
       </c>
       <c r="B117" s="4" t="n">
-        <v>15.46</v>
+        <v>9.359999999999999</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B118" s="4" t="n">
+        <v>9.51</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B119" s="4" t="n">
+        <v>9.57</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="A120" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B120" s="4" t="n">
+        <v>10.28</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B121" s="4" t="n">
+        <v>11.78</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B122" s="4" t="n">
+        <v>13.06</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="A123" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B123" s="4" t="n">
+        <v>14.32</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="A124" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B124" s="4" t="n">
+        <v>15.64</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B125" s="4" t="n">
+        <v>17.38</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
+      <c r="A126" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B126" s="4" t="n">
+        <v>19.9</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="A127" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B127" s="4" t="n">
+        <v>22.04</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="A128" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B128" s="4" t="n">
+        <v>24.24</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B129" s="4" t="n">
+        <v>26.79</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B130" s="4" t="n">
+        <v>30.08</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B131" s="4" t="n">
+        <v>32.12</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
+      <c r="A132" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B132" s="4" t="n">
+        <v>34.23</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
+      <c r="A133" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B133" s="4" t="n">
+        <v>35.69</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B134" s="4" t="n">
+        <v>36.91</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="A135" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B135" s="4" t="n">
+        <v>37.32</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="A136" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B136" s="4" t="n">
+        <v>36.94</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="A137" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B137" s="4" t="n">
+        <v>36.78</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B138" s="4" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="A139" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B139" s="4" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
+      <c r="A140" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B140" s="4" t="n">
+        <v>35.3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
+      <c r="A141" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B141" s="4" t="n">
+        <v>33.73</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4">
+      <c r="A142" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B142" s="4" t="n">
+        <v>32.41</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4">
+      <c r="A143" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B143" s="4" t="n">
+        <v>31.09</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
+      <c r="A144" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B144" s="4" t="n">
+        <v>29.92</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
+      <c r="A145" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B145" s="4" t="n">
+        <v>29.38</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
+      <c r="A146" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B146" s="4" t="n">
+        <v>29.29</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
+      <c r="A147" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B147" s="4" t="n">
+        <v>32.03</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4">
+      <c r="A148" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B148" s="4" t="n">
+        <v>33.03</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
+      <c r="A149" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B149" s="4" t="n">
+        <v>33.79</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4">
+      <c r="A150" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B150" s="4" t="n">
+        <v>34.03</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4">
+      <c r="A151" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B151" s="4" t="n">
+        <v>34.73</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4">
+      <c r="A152" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B152" s="4" t="n">
+        <v>35.19</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4">
+      <c r="A153" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B153" s="4" t="n">
+        <v>36.45</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4">
+      <c r="A154" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B154" s="4" t="n">
+        <v>37.33</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4">
+      <c r="A155" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B155" s="4" t="n">
+        <v>37.73</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4">
+      <c r="A156" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B156" s="4" t="n">
+        <v>37.44</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4">
+      <c r="A157" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B157" s="4" t="n">
+        <v>34.36</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4">
+      <c r="A158" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B158" s="4" t="n">
+        <v>31.87</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4">
+      <c r="A159" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B159" s="4" t="n">
+        <v>29.86</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4">
+      <c r="A160" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B160" s="4" t="n">
+        <v>29.09</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4">
+      <c r="A161" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B161" s="4" t="n">
+        <v>27.74</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4">
+      <c r="A162" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B162" s="4" t="n">
+        <v>26.85</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4">
+      <c r="A163" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B163" s="4" t="n">
+        <v>25.33</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4">
+      <c r="A164" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B164" s="4" t="n">
+        <v>23.73</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4">
+      <c r="A165" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B165" s="4" t="n">
+        <v>22.47</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4">
+      <c r="A166" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B166" s="4" t="n">
+        <v>21.04</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4">
+      <c r="A167" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B167" s="4" t="n">
+        <v>19.89</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4">
+      <c r="A168" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B168" s="4" t="n">
+        <v>19.74</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4">
+      <c r="A169" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B169" s="4" t="n">
+        <v>19.65</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4">
+      <c r="A170" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B170" s="4" t="n">
+        <v>18.81</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4">
+      <c r="A171" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B171" s="4" t="n">
+        <v>19.19</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4">
+      <c r="A172" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B172" s="4" t="n">
+        <v>18.97</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4">
+      <c r="A173" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B173" s="4" t="n">
+        <v>19.28</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4">
+      <c r="A174" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B174" s="4" t="n">
+        <v>20.18</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4">
+      <c r="A175" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B175" s="4" t="n">
+        <v>20.86</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4">
+      <c r="A176" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B176" s="4" t="n">
+        <v>21.39</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4">
+      <c r="A177" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B177" s="4" t="n">
+        <v>21.45</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4">
+      <c r="A178" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B178" s="4" t="n">
+        <v>21.23</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4">
+      <c r="A179" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B179" s="4" t="n">
+        <v>20.83</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4">
+      <c r="A180" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B180" s="4" t="n">
+        <v>21.02</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4">
+      <c r="A181" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B181" s="4" t="n">
+        <v>21.03</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4">
+      <c r="A182" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B182" s="4" t="n">
+        <v>20.24</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4">
+      <c r="A183" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B183" s="4" t="n">
+        <v>19.31</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4">
+      <c r="A184" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B184" s="4" t="n">
+        <v>18.23</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4">
+      <c r="A185" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B185" s="4" t="n">
+        <v>17.12</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4">
+      <c r="A186" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B186" s="4" t="n">
+        <v>16.56</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4">
+      <c r="A187" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B187" s="4" t="n">
+        <v>16.76</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4">
+      <c r="A188" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B188" s="4" t="n">
+        <v>16.09</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4">
+      <c r="A189" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B189" s="4" t="n">
+        <v>15.04</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4">
+      <c r="A190" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B190" s="4" t="n">
+        <v>13.74</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4">
+      <c r="A191" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B191" s="4" t="n">
+        <v>12.17</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4">
+      <c r="A192" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B192" s="4" t="n">
+        <v>12.46</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4">
+      <c r="A193" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B193" s="4" t="n">
+        <v>14.41</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4">
+      <c r="A194" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B194" s="4" t="n">
+        <v>16.55</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4">
+      <c r="A195" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B195" s="4" t="n">
+        <v>19.71</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4">
+      <c r="A196" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B196" s="4" t="n">
+        <v>23.61</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4">
+      <c r="A197" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B197" s="4" t="n">
+        <v>28.44</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4">
+      <c r="A198" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B198" s="4" t="n">
+        <v>33.98</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4">
+      <c r="A199" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B199" s="4" t="n">
+        <v>38.54</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4">
+      <c r="A200" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B200" s="4" t="n">
+        <v>41.92</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4">
+      <c r="A201" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B201" s="4" t="n">
+        <v>43.55</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4">
+      <c r="A202" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B202" s="4" t="n">
+        <v>50.28</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4">
+      <c r="A203" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B203" s="4" t="n">
+        <v>55.27</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4">
+      <c r="A204" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B204" s="4" t="n">
+        <v>60.75</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4">
+      <c r="A205" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B205" s="4" t="n">
+        <v>65.18000000000001</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4">
+      <c r="A206" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B206" s="4" t="n">
+        <v>68.44</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4">
+      <c r="A207" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B207" s="4" t="n">
+        <v>68.28</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4">
+      <c r="A208" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B208" s="4" t="n">
+        <v>65.97</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4">
+      <c r="A209" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B209" s="4" t="n">
+        <v>65.72</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4">
+      <c r="A210" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B210" s="4" t="n">
+        <v>64.68000000000001</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4">
+      <c r="A211" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B211" s="4" t="n">
+        <v>66.23999999999999</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4">
+      <c r="A212" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B212" s="4" t="n">
+        <v>63.85</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4">
+      <c r="A213" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B213" s="4" t="n">
+        <v>63.9</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4">
+      <c r="A214" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B214" s="4" t="n">
+        <v>63.09</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4">
+      <c r="A215" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="B215" s="4" t="n">
+        <v>60.47</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4">
+      <c r="A216" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B216" s="4" t="n">
+        <v>58.51</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4">
+      <c r="A217" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B217" s="4" t="n">
+        <v>63.79</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4">
+      <c r="A218" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="B218" s="4" t="n">
+        <v>68.63</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4">
+      <c r="A219" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B219" s="4" t="n">
+        <v>71.83</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4">
+      <c r="A220" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B220" s="4" t="n">
+        <v>74.94</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4">
+      <c r="A221" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B221" s="4" t="n">
+        <v>74.34999999999999</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4">
+      <c r="A222" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="B222" s="4" t="n">
+        <v>73.01000000000001</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4">
+      <c r="A223" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="B223" s="4" t="n">
+        <v>68.17</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4">
+      <c r="A224" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="B224" s="4" t="n">
+        <v>62.25</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4">
+      <c r="A225" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B225" s="4" t="n">
+        <v>58.14</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4">
+      <c r="A226" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="B226" s="4" t="n">
+        <v>54.55</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4">
+      <c r="A227" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="B227" s="4" t="n">
+        <v>44.82</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4">
+      <c r="A228" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B228" s="4" t="n">
+        <v>37.48</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4">
+      <c r="A229" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B229" s="4" t="n">
+        <v>30.81</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4">
+      <c r="A230" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="B230" s="4" t="n">
+        <v>26.25</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4">
+      <c r="A231" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="B231" s="4" t="n">
+        <v>24.65</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4">
+      <c r="A232" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="B232" s="4" t="n">
+        <v>22.18</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4">
+      <c r="A233" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="B233" s="4" t="n">
+        <v>20.61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>